<commit_message>
Testing for Patch 2 V3
</commit_message>
<xml_diff>
--- a/python_files/test_side_by_side/AARF_vs_SmartV3/AARF_vs_SmartV3_comparison.xlsx
+++ b/python_files/test_side_by_side/AARF_vs_SmartV3/AARF_vs_SmartV3_comparison.xlsx
@@ -4641,7 +4641,7 @@
         <v>0</v>
       </c>
       <c r="I80" t="n">
-        <v>0.113083</v>
+        <v>0.11315</v>
       </c>
       <c r="J80" t="n">
         <v>3906</v>
@@ -4797,7 +4797,7 @@
         <v>0</v>
       </c>
       <c r="I83" t="n">
-        <v>0.344521</v>
+        <v>0.341728</v>
       </c>
       <c r="J83" t="n">
         <v>666</v>
@@ -4901,7 +4901,7 @@
         <v>3.85</v>
       </c>
       <c r="I85" t="n">
-        <v>387.104</v>
+        <v>386.934</v>
       </c>
       <c r="J85" t="n">
         <v>34614</v>
@@ -4953,7 +4953,7 @@
         <v>86.9944</v>
       </c>
       <c r="I86" t="n">
-        <v>0.2652</v>
+        <v>0.248265</v>
       </c>
       <c r="J86" t="n">
         <v>508</v>
@@ -4999,16 +4999,16 @@
         </is>
       </c>
       <c r="G87" t="n">
-        <v>0.761688</v>
+        <v>0.77532</v>
       </c>
       <c r="H87" t="n">
-        <v>87.5163</v>
+        <v>87.2929</v>
       </c>
       <c r="I87" t="n">
-        <v>148.909</v>
+        <v>146.397</v>
       </c>
       <c r="J87" t="n">
-        <v>5364</v>
+        <v>5460</v>
       </c>
       <c r="K87" t="n">
         <v>42968</v>
@@ -5051,16 +5051,16 @@
         </is>
       </c>
       <c r="G88" t="n">
-        <v>1.1671</v>
+        <v>1.16284</v>
       </c>
       <c r="H88" t="n">
-        <v>96.1036</v>
+        <v>96.1178</v>
       </c>
       <c r="I88" t="n">
-        <v>839.539</v>
+        <v>837.028</v>
       </c>
       <c r="J88" t="n">
-        <v>8219</v>
+        <v>8189</v>
       </c>
       <c r="K88" t="n">
         <v>210937</v>
@@ -5109,7 +5109,7 @@
         <v>86.93689999999999</v>
       </c>
       <c r="I89" t="n">
-        <v>0.962311</v>
+        <v>0.936518</v>
       </c>
       <c r="J89" t="n">
         <v>87</v>
@@ -5155,16 +5155,16 @@
         </is>
       </c>
       <c r="G90" t="n">
-        <v>0.711284</v>
+        <v>0.7288559999999999</v>
       </c>
       <c r="H90" t="n">
-        <v>87.304</v>
+        <v>86.9903</v>
       </c>
       <c r="I90" t="n">
-        <v>1.51198</v>
+        <v>1.28894</v>
       </c>
       <c r="J90" t="n">
-        <v>931</v>
+        <v>954</v>
       </c>
       <c r="K90" t="n">
         <v>7333</v>
@@ -5207,16 +5207,16 @@
         </is>
       </c>
       <c r="G91" t="n">
-        <v>2.77256</v>
+        <v>2.75269</v>
       </c>
       <c r="H91" t="n">
-        <v>89.9194</v>
+        <v>89.99169999999999</v>
       </c>
       <c r="I91" t="n">
-        <v>577.1</v>
+        <v>574.172</v>
       </c>
       <c r="J91" t="n">
-        <v>3629</v>
+        <v>3603</v>
       </c>
       <c r="K91" t="n">
         <v>36000</v>
@@ -5265,7 +5265,7 @@
         <v>87.02</v>
       </c>
       <c r="I92" t="n">
-        <v>0.521926</v>
+        <v>0.485469</v>
       </c>
       <c r="J92" t="n">
         <v>507</v>
@@ -5311,16 +5311,16 @@
         </is>
       </c>
       <c r="G93" t="n">
-        <v>0.365508</v>
+        <v>0.399162</v>
       </c>
       <c r="H93" t="n">
-        <v>94.0095</v>
+        <v>93.4579</v>
       </c>
       <c r="I93" t="n">
-        <v>541.864</v>
+        <v>543.3869999999999</v>
       </c>
       <c r="J93" t="n">
-        <v>2574</v>
+        <v>2811</v>
       </c>
       <c r="K93" t="n">
         <v>42968</v>
@@ -5363,16 +5363,16 @@
         </is>
       </c>
       <c r="G94" t="n">
-        <v>0.375874</v>
+        <v>0.440058</v>
       </c>
       <c r="H94" t="n">
-        <v>98.74509999999999</v>
+        <v>98.5308</v>
       </c>
       <c r="I94" t="n">
-        <v>756.564</v>
+        <v>748.5549999999999</v>
       </c>
       <c r="J94" t="n">
-        <v>2647</v>
+        <v>3099</v>
       </c>
       <c r="K94" t="n">
         <v>210937</v>
@@ -5421,7 +5421,7 @@
         <v>86.93689999999999</v>
       </c>
       <c r="I95" t="n">
-        <v>1.3949</v>
+        <v>1.34131</v>
       </c>
       <c r="J95" t="n">
         <v>87</v>
@@ -5467,16 +5467,16 @@
         </is>
       </c>
       <c r="G96" t="n">
-        <v>0.650928</v>
+        <v>0.696004</v>
       </c>
       <c r="H96" t="n">
-        <v>88.3813</v>
+        <v>87.5767</v>
       </c>
       <c r="I96" t="n">
-        <v>98.24550000000001</v>
+        <v>112.863</v>
       </c>
       <c r="J96" t="n">
-        <v>852</v>
+        <v>911</v>
       </c>
       <c r="K96" t="n">
         <v>7333</v>
@@ -5519,16 +5519,16 @@
         </is>
       </c>
       <c r="G97" t="n">
-        <v>0.854916</v>
+        <v>0.738788</v>
       </c>
       <c r="H97" t="n">
-        <v>96.8917</v>
+        <v>97.3139</v>
       </c>
       <c r="I97" t="n">
-        <v>534.5170000000001</v>
+        <v>340.181</v>
       </c>
       <c r="J97" t="n">
-        <v>1119</v>
+        <v>967</v>
       </c>
       <c r="K97" t="n">
         <v>36000</v>
@@ -5889,7 +5889,7 @@
         <v>0.0256016</v>
       </c>
       <c r="I104" t="n">
-        <v>0.435999</v>
+        <v>0.35478</v>
       </c>
       <c r="J104" t="n">
         <v>3905</v>
@@ -5935,16 +5935,16 @@
         </is>
       </c>
       <c r="G105" t="n">
-        <v>5.11598</v>
+        <v>5.52849</v>
       </c>
       <c r="H105" t="n">
-        <v>16.1516</v>
+        <v>9.39071</v>
       </c>
       <c r="I105" t="n">
-        <v>1531.3</v>
+        <v>711.768</v>
       </c>
       <c r="J105" t="n">
-        <v>36028</v>
+        <v>38933</v>
       </c>
       <c r="K105" t="n">
         <v>42968</v>
@@ -5987,16 +5987,16 @@
         </is>
       </c>
       <c r="G106" t="n">
-        <v>5.10689</v>
+        <v>5.76548</v>
       </c>
       <c r="H106" t="n">
-        <v>82.9504</v>
+        <v>80.7516</v>
       </c>
       <c r="I106" t="n">
-        <v>3474.08</v>
+        <v>3153.3</v>
       </c>
       <c r="J106" t="n">
-        <v>35964</v>
+        <v>40602</v>
       </c>
       <c r="K106" t="n">
         <v>210937</v>
@@ -6045,7 +6045,7 @@
         <v>0</v>
       </c>
       <c r="I107" t="n">
-        <v>1.40879</v>
+        <v>1.14079</v>
       </c>
       <c r="J107" t="n">
         <v>666</v>
@@ -6091,16 +6091,16 @@
         </is>
       </c>
       <c r="G108" t="n">
-        <v>5.23569</v>
+        <v>5.59401</v>
       </c>
       <c r="H108" t="n">
-        <v>6.54575</v>
+        <v>0.150007</v>
       </c>
       <c r="I108" t="n">
-        <v>347.843</v>
+        <v>234.004</v>
       </c>
       <c r="J108" t="n">
-        <v>6853</v>
+        <v>7322</v>
       </c>
       <c r="K108" t="n">
         <v>7333</v>
@@ -6143,16 +6143,16 @@
         </is>
       </c>
       <c r="G109" t="n">
-        <v>9.076320000000001</v>
+        <v>10.7472</v>
       </c>
       <c r="H109" t="n">
-        <v>67</v>
+        <v>60.925</v>
       </c>
       <c r="I109" t="n">
-        <v>4168.01</v>
+        <v>4128.21</v>
       </c>
       <c r="J109" t="n">
-        <v>11880</v>
+        <v>14067</v>
       </c>
       <c r="K109" t="n">
         <v>36000</v>
@@ -8144,10 +8144,10 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>4.6843</v>
+        <v>4.7705</v>
       </c>
       <c r="D4" t="n">
-        <v>6.9987</v>
+        <v>7.0378</v>
       </c>
       <c r="E4" t="n">
         <v>36</v>
@@ -8163,10 +8163,10 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.2205</v>
+        <v>0.2214</v>
       </c>
       <c r="D5" t="n">
-        <v>0.5301</v>
+        <v>0.5264</v>
       </c>
       <c r="E5" t="n">
         <v>36</v>
@@ -8273,10 +8273,10 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>44.5266</v>
+        <v>43.9313</v>
       </c>
       <c r="D4" t="n">
-        <v>45.8133</v>
+        <v>45.9823</v>
       </c>
       <c r="E4" t="n">
         <v>36</v>
@@ -8292,10 +8292,10 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>96.8544</v>
+        <v>96.81</v>
       </c>
       <c r="D5" t="n">
-        <v>5.1787</v>
+        <v>5.251</v>
       </c>
       <c r="E5" t="n">
         <v>36</v>
@@ -8323,7 +8323,7 @@
     <col width="10" customWidth="1" min="1" max="1"/>
     <col width="7" customWidth="1" min="2" max="2"/>
     <col width="10" customWidth="1" min="3" max="3"/>
-    <col width="11" customWidth="1" min="4" max="4"/>
+    <col width="10" customWidth="1" min="4" max="4"/>
     <col width="7" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
@@ -8402,10 +8402,10 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>485.9856</v>
+        <v>450.028</v>
       </c>
       <c r="D4" t="n">
-        <v>1003.5779</v>
+        <v>957.7024</v>
       </c>
       <c r="E4" t="n">
         <v>36</v>
@@ -8421,10 +8421,10 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>97.261</v>
+        <v>91.8579</v>
       </c>
       <c r="D5" t="n">
-        <v>231.8168</v>
+        <v>222.4556</v>
       </c>
       <c r="E5" t="n">
         <v>36</v>
@@ -8531,10 +8531,10 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>2.7273</v>
+        <v>2.7275</v>
       </c>
       <c r="D4" t="n">
-        <v>5.8312</v>
+        <v>5.8309</v>
       </c>
       <c r="E4" t="n">
         <v>36</v>
@@ -8550,10 +8550,10 @@
         <v>3</v>
       </c>
       <c r="C5" t="n">
-        <v>2.1775</v>
+        <v>2.2644</v>
       </c>
       <c r="D5" t="n">
-        <v>5.035</v>
+        <v>5.1323</v>
       </c>
       <c r="E5" t="n">
         <v>36</v>
@@ -8660,10 +8660,10 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>69.4007</v>
+        <v>69.3882</v>
       </c>
       <c r="D4" t="n">
-        <v>42.6162</v>
+        <v>42.611</v>
       </c>
       <c r="E4" t="n">
         <v>36</v>
@@ -8679,10 +8679,10 @@
         <v>3</v>
       </c>
       <c r="C5" t="n">
-        <v>71.9804</v>
+        <v>71.3532</v>
       </c>
       <c r="D5" t="n">
-        <v>41.4045</v>
+        <v>41.9796</v>
       </c>
       <c r="E5" t="n">
         <v>36</v>
@@ -8789,10 +8789,10 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>204.4302</v>
+        <v>204.2019</v>
       </c>
       <c r="D4" t="n">
-        <v>487.2522</v>
+        <v>487.1066</v>
       </c>
       <c r="E4" t="n">
         <v>36</v>
@@ -8808,10 +8808,10 @@
         <v>3</v>
       </c>
       <c r="C5" t="n">
-        <v>378.8164</v>
+        <v>337.684</v>
       </c>
       <c r="D5" t="n">
-        <v>941.0447</v>
+        <v>886.6904</v>
       </c>
       <c r="E5" t="n">
         <v>36</v>
@@ -8918,10 +8918,10 @@
         <v>256</v>
       </c>
       <c r="C4" t="n">
-        <v>1.7997</v>
+        <v>1.8325</v>
       </c>
       <c r="D4" t="n">
-        <v>3.2855</v>
+        <v>3.3174</v>
       </c>
       <c r="E4" t="n">
         <v>36</v>
@@ -8937,10 +8937,10 @@
         <v>1500</v>
       </c>
       <c r="C5" t="n">
-        <v>3.1051</v>
+        <v>3.1594</v>
       </c>
       <c r="D5" t="n">
-        <v>6.9166</v>
+        <v>6.9671</v>
       </c>
       <c r="E5" t="n">
         <v>36</v>
@@ -9047,10 +9047,10 @@
         <v>256</v>
       </c>
       <c r="C4" t="n">
-        <v>73.5245</v>
+        <v>73.24850000000001</v>
       </c>
       <c r="D4" t="n">
-        <v>39.9588</v>
+        <v>40.2238</v>
       </c>
       <c r="E4" t="n">
         <v>36</v>
@@ -9066,10 +9066,10 @@
         <v>1500</v>
       </c>
       <c r="C5" t="n">
-        <v>67.8566</v>
+        <v>67.4928</v>
       </c>
       <c r="D5" t="n">
-        <v>43.8254</v>
+        <v>44.1019</v>
       </c>
       <c r="E5" t="n">
         <v>36</v>
@@ -9176,10 +9176,10 @@
         <v>256</v>
       </c>
       <c r="C4" t="n">
-        <v>366.2996</v>
+        <v>334.3009</v>
       </c>
       <c r="D4" t="n">
-        <v>782.7824000000001</v>
+        <v>722.5688</v>
       </c>
       <c r="E4" t="n">
         <v>36</v>
@@ -9195,10 +9195,10 @@
         <v>1500</v>
       </c>
       <c r="C5" t="n">
-        <v>216.9469</v>
+        <v>207.585</v>
       </c>
       <c r="D5" t="n">
-        <v>717.2166</v>
+        <v>708.7259</v>
       </c>
       <c r="E5" t="n">
         <v>36</v>
@@ -9332,10 +9332,10 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1.9926</v>
+        <v>2.0293</v>
       </c>
       <c r="D5" t="n">
-        <v>2.6719</v>
+        <v>2.7112</v>
       </c>
       <c r="E5" t="n">
         <v>24</v>
@@ -9374,10 +9374,10 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>5.1759</v>
+        <v>5.2698</v>
       </c>
       <c r="D7" t="n">
-        <v>8.3696</v>
+        <v>8.4123</v>
       </c>
       <c r="E7" t="n">
         <v>24</v>
@@ -12774,10 +12774,10 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>65.92</v>
+        <v>65.2929</v>
       </c>
       <c r="D5" t="n">
-        <v>45.657</v>
+        <v>46.3284</v>
       </c>
       <c r="E5" t="n">
         <v>24</v>
@@ -12816,10 +12816,10 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>81.652</v>
+        <v>81.31950000000001</v>
       </c>
       <c r="D7" t="n">
-        <v>30.2021</v>
+        <v>30.3591</v>
       </c>
       <c r="E7" t="n">
         <v>24</v>
@@ -12847,7 +12847,7 @@
     <col width="10" customWidth="1" min="1" max="1"/>
     <col width="14" customWidth="1" min="2" max="2"/>
     <col width="10" customWidth="1" min="3" max="3"/>
-    <col width="11" customWidth="1" min="4" max="4"/>
+    <col width="10" customWidth="1" min="4" max="4"/>
     <col width="7" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
@@ -12953,10 +12953,10 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>126.37</v>
+        <v>88.0381</v>
       </c>
       <c r="D5" t="n">
-        <v>326.6548</v>
+        <v>180.6893</v>
       </c>
       <c r="E5" t="n">
         <v>24</v>
@@ -12974,10 +12974,10 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.279</v>
+        <v>0.2588</v>
       </c>
       <c r="D6" t="n">
-        <v>0.4252</v>
+        <v>0.3861</v>
       </c>
       <c r="E6" t="n">
         <v>24</v>
@@ -12995,10 +12995,10 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>748.2209</v>
+        <v>724.532</v>
       </c>
       <c r="D7" t="n">
-        <v>1136.3823</v>
+        <v>1101.241</v>
       </c>
       <c r="E7" t="n">
         <v>24</v>
@@ -13091,7 +13091,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-08-17 12:21:44</t>
+          <t>2025-08-17 12:32:34</t>
         </is>
       </c>
     </row>
@@ -13506,7 +13506,7 @@
         <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>0.113083</v>
+        <v>0.11315</v>
       </c>
       <c r="J8" t="n">
         <v>3906</v>
@@ -13638,7 +13638,7 @@
         <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>0.344521</v>
+        <v>0.341728</v>
       </c>
       <c r="J11" t="n">
         <v>666</v>
@@ -13726,7 +13726,7 @@
         <v>3.85</v>
       </c>
       <c r="I13" t="n">
-        <v>387.104</v>
+        <v>386.934</v>
       </c>
       <c r="J13" t="n">
         <v>34614</v>
@@ -13770,7 +13770,7 @@
         <v>86.9944</v>
       </c>
       <c r="I14" t="n">
-        <v>0.2652</v>
+        <v>0.248265</v>
       </c>
       <c r="J14" t="n">
         <v>508</v>
@@ -13808,16 +13808,16 @@
         </is>
       </c>
       <c r="G15" t="n">
-        <v>0.761688</v>
+        <v>0.77532</v>
       </c>
       <c r="H15" t="n">
-        <v>87.5163</v>
+        <v>87.2929</v>
       </c>
       <c r="I15" t="n">
-        <v>148.909</v>
+        <v>146.397</v>
       </c>
       <c r="J15" t="n">
-        <v>5364</v>
+        <v>5460</v>
       </c>
       <c r="K15" t="n">
         <v>42968</v>
@@ -13852,16 +13852,16 @@
         </is>
       </c>
       <c r="G16" t="n">
-        <v>1.1671</v>
+        <v>1.16284</v>
       </c>
       <c r="H16" t="n">
-        <v>96.1036</v>
+        <v>96.1178</v>
       </c>
       <c r="I16" t="n">
-        <v>839.539</v>
+        <v>837.028</v>
       </c>
       <c r="J16" t="n">
-        <v>8219</v>
+        <v>8189</v>
       </c>
       <c r="K16" t="n">
         <v>210937</v>
@@ -13902,7 +13902,7 @@
         <v>86.93689999999999</v>
       </c>
       <c r="I17" t="n">
-        <v>0.962311</v>
+        <v>0.936518</v>
       </c>
       <c r="J17" t="n">
         <v>87</v>
@@ -13940,16 +13940,16 @@
         </is>
       </c>
       <c r="G18" t="n">
-        <v>0.711284</v>
+        <v>0.7288559999999999</v>
       </c>
       <c r="H18" t="n">
-        <v>87.304</v>
+        <v>86.9903</v>
       </c>
       <c r="I18" t="n">
-        <v>1.51198</v>
+        <v>1.28894</v>
       </c>
       <c r="J18" t="n">
-        <v>931</v>
+        <v>954</v>
       </c>
       <c r="K18" t="n">
         <v>7333</v>
@@ -13984,16 +13984,16 @@
         </is>
       </c>
       <c r="G19" t="n">
-        <v>2.77256</v>
+        <v>2.75269</v>
       </c>
       <c r="H19" t="n">
-        <v>89.9194</v>
+        <v>89.99169999999999</v>
       </c>
       <c r="I19" t="n">
-        <v>577.1</v>
+        <v>574.172</v>
       </c>
       <c r="J19" t="n">
-        <v>3629</v>
+        <v>3603</v>
       </c>
       <c r="K19" t="n">
         <v>36000</v>
@@ -14034,7 +14034,7 @@
         <v>87.02</v>
       </c>
       <c r="I20" t="n">
-        <v>0.521926</v>
+        <v>0.485469</v>
       </c>
       <c r="J20" t="n">
         <v>507</v>
@@ -14072,16 +14072,16 @@
         </is>
       </c>
       <c r="G21" t="n">
-        <v>0.365508</v>
+        <v>0.399162</v>
       </c>
       <c r="H21" t="n">
-        <v>94.0095</v>
+        <v>93.4579</v>
       </c>
       <c r="I21" t="n">
-        <v>541.864</v>
+        <v>543.3869999999999</v>
       </c>
       <c r="J21" t="n">
-        <v>2574</v>
+        <v>2811</v>
       </c>
       <c r="K21" t="n">
         <v>42968</v>
@@ -14116,16 +14116,16 @@
         </is>
       </c>
       <c r="G22" t="n">
-        <v>0.375874</v>
+        <v>0.440058</v>
       </c>
       <c r="H22" t="n">
-        <v>98.74509999999999</v>
+        <v>98.5308</v>
       </c>
       <c r="I22" t="n">
-        <v>756.564</v>
+        <v>748.5549999999999</v>
       </c>
       <c r="J22" t="n">
-        <v>2647</v>
+        <v>3099</v>
       </c>
       <c r="K22" t="n">
         <v>210937</v>
@@ -14166,7 +14166,7 @@
         <v>86.93689999999999</v>
       </c>
       <c r="I23" t="n">
-        <v>1.3949</v>
+        <v>1.34131</v>
       </c>
       <c r="J23" t="n">
         <v>87</v>
@@ -14204,16 +14204,16 @@
         </is>
       </c>
       <c r="G24" t="n">
-        <v>0.650928</v>
+        <v>0.696004</v>
       </c>
       <c r="H24" t="n">
-        <v>88.3813</v>
+        <v>87.5767</v>
       </c>
       <c r="I24" t="n">
-        <v>98.24550000000001</v>
+        <v>112.863</v>
       </c>
       <c r="J24" t="n">
-        <v>852</v>
+        <v>911</v>
       </c>
       <c r="K24" t="n">
         <v>7333</v>
@@ -14248,16 +14248,16 @@
         </is>
       </c>
       <c r="G25" t="n">
-        <v>0.854916</v>
+        <v>0.738788</v>
       </c>
       <c r="H25" t="n">
-        <v>96.8917</v>
+        <v>97.3139</v>
       </c>
       <c r="I25" t="n">
-        <v>534.5170000000001</v>
+        <v>340.181</v>
       </c>
       <c r="J25" t="n">
-        <v>1119</v>
+        <v>967</v>
       </c>
       <c r="K25" t="n">
         <v>36000</v>
@@ -14562,7 +14562,7 @@
         <v>0.0256016</v>
       </c>
       <c r="I32" t="n">
-        <v>0.435999</v>
+        <v>0.35478</v>
       </c>
       <c r="J32" t="n">
         <v>3905</v>
@@ -14600,16 +14600,16 @@
         </is>
       </c>
       <c r="G33" t="n">
-        <v>5.11598</v>
+        <v>5.52849</v>
       </c>
       <c r="H33" t="n">
-        <v>16.1516</v>
+        <v>9.39071</v>
       </c>
       <c r="I33" t="n">
-        <v>1531.3</v>
+        <v>711.768</v>
       </c>
       <c r="J33" t="n">
-        <v>36028</v>
+        <v>38933</v>
       </c>
       <c r="K33" t="n">
         <v>42968</v>
@@ -14644,16 +14644,16 @@
         </is>
       </c>
       <c r="G34" t="n">
-        <v>5.10689</v>
+        <v>5.76548</v>
       </c>
       <c r="H34" t="n">
-        <v>82.9504</v>
+        <v>80.7516</v>
       </c>
       <c r="I34" t="n">
-        <v>3474.08</v>
+        <v>3153.3</v>
       </c>
       <c r="J34" t="n">
-        <v>35964</v>
+        <v>40602</v>
       </c>
       <c r="K34" t="n">
         <v>210937</v>
@@ -14694,7 +14694,7 @@
         <v>0</v>
       </c>
       <c r="I35" t="n">
-        <v>1.40879</v>
+        <v>1.14079</v>
       </c>
       <c r="J35" t="n">
         <v>666</v>
@@ -14732,16 +14732,16 @@
         </is>
       </c>
       <c r="G36" t="n">
-        <v>5.23569</v>
+        <v>5.59401</v>
       </c>
       <c r="H36" t="n">
-        <v>6.54575</v>
+        <v>0.150007</v>
       </c>
       <c r="I36" t="n">
-        <v>347.843</v>
+        <v>234.004</v>
       </c>
       <c r="J36" t="n">
-        <v>6853</v>
+        <v>7322</v>
       </c>
       <c r="K36" t="n">
         <v>7333</v>
@@ -14776,16 +14776,16 @@
         </is>
       </c>
       <c r="G37" t="n">
-        <v>9.076320000000001</v>
+        <v>10.7472</v>
       </c>
       <c r="H37" t="n">
-        <v>67</v>
+        <v>60.925</v>
       </c>
       <c r="I37" t="n">
-        <v>4168.01</v>
+        <v>4128.21</v>
       </c>
       <c r="J37" t="n">
-        <v>11880</v>
+        <v>14067</v>
       </c>
       <c r="K37" t="n">
         <v>36000</v>
@@ -16477,10 +16477,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2.4524</v>
+        <v>2.4959</v>
       </c>
       <c r="C3" t="n">
-        <v>5.4163</v>
+        <v>5.4589</v>
       </c>
       <c r="D3" t="n">
         <v>0.0332</v>
@@ -16516,7 +16516,7 @@
   <cols>
     <col width="10" customWidth="1" min="1" max="1"/>
     <col width="9" customWidth="1" min="2" max="2"/>
-    <col width="8" customWidth="1" min="3" max="3"/>
+    <col width="9" customWidth="1" min="3" max="3"/>
     <col width="9" customWidth="1" min="4" max="4"/>
     <col width="5" customWidth="1" min="5" max="5"/>
     <col width="5" customWidth="1" min="6" max="6"/>
@@ -16592,13 +16592,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>70.6905</v>
+        <v>70.3707</v>
       </c>
       <c r="C3" t="n">
-        <v>41.738</v>
+        <v>42.0092</v>
       </c>
       <c r="D3" t="n">
-        <v>99.3725</v>
+        <v>99.2654</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -16707,19 +16707,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>291.6233</v>
+        <v>270.9429</v>
       </c>
       <c r="C3" t="n">
-        <v>749.1938</v>
+        <v>713.4814</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0565</v>
+        <v>0.0566</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>4168.01</v>
+        <v>4128.21</v>
       </c>
       <c r="G3" t="n">
         <v>72</v>
@@ -16845,10 +16845,10 @@
         <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>4.3617</v>
+        <v>4.3631</v>
       </c>
       <c r="D5" t="n">
-        <v>7.1426</v>
+        <v>7.1414</v>
       </c>
       <c r="E5" t="n">
         <v>24</v>
@@ -16864,10 +16864,10 @@
         <v>40</v>
       </c>
       <c r="C6" t="n">
-        <v>2.9955</v>
+        <v>3.1247</v>
       </c>
       <c r="D6" t="n">
-        <v>5.3994</v>
+        <v>5.5172</v>
       </c>
       <c r="E6" t="n">
         <v>24</v>
@@ -17012,10 +17012,10 @@
         <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>51.4615</v>
+        <v>51.3948</v>
       </c>
       <c r="D5" t="n">
-        <v>43.5532</v>
+        <v>43.4938</v>
       </c>
       <c r="E5" t="n">
         <v>24</v>
@@ -17031,10 +17031,10 @@
         <v>40</v>
       </c>
       <c r="C6" t="n">
-        <v>60.6101</v>
+        <v>59.7172</v>
       </c>
       <c r="D6" t="n">
-        <v>45.7441</v>
+        <v>46.3231</v>
       </c>
       <c r="E6" t="n">
         <v>24</v>
@@ -17179,10 +17179,10 @@
         <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>357.3059</v>
+        <v>349.1941</v>
       </c>
       <c r="D5" t="n">
-        <v>536.4104</v>
+        <v>534.4529</v>
       </c>
       <c r="E5" t="n">
         <v>24</v>
@@ -17198,10 +17198,10 @@
         <v>40</v>
       </c>
       <c r="C6" t="n">
-        <v>517.5639</v>
+        <v>463.6347</v>
       </c>
       <c r="D6" t="n">
-        <v>1139.4884</v>
+        <v>1078.9149</v>
       </c>
       <c r="E6" t="n">
         <v>24</v>

</xml_diff>